<commit_message>
Updated and corrected notes and instructions, added a rubric
</commit_message>
<xml_diff>
--- a/LabStarters/Lab06/Lab6Rubric-CIS195.xlsx
+++ b/LabStarters/Lab06/Lab6Rubric-CIS195.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/birdb/Projects/CIS195-CourseMaterials/LabStarters/Lab06/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DataCard/Repos/CIS195-CourseMaterials/LabStarters/Lab06/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CADE662A-EFB5-1E4F-894C-B905288C1426}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C8D7005D-96B5-E24B-89C1-62C87A8D8F9C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21180" yWindow="2880" windowWidth="20920" windowHeight="22120" xr2:uid="{5D75B731-65CD-014E-8BBA-DE69945DF98D}"/>
+    <workbookView xWindow="5960" yWindow="500" windowWidth="20920" windowHeight="16500" xr2:uid="{5D75B731-65CD-014E-8BBA-DE69945DF98D}"/>
   </bookViews>
   <sheets>
     <sheet name="Rubric" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="32">
   <si>
     <t>Requirements:</t>
   </si>
@@ -40,9 +40,6 @@
     <t>Total:</t>
   </si>
   <si>
-    <t>Total</t>
-  </si>
-  <si>
     <t>Syntax and Style are correct</t>
   </si>
   <si>
@@ -110,6 +107,21 @@
   </si>
   <si>
     <t>Syntax and style</t>
+  </si>
+  <si>
+    <t>Eight events, each on a different day</t>
+  </si>
+  <si>
+    <t>Subtotal:</t>
+  </si>
+  <si>
+    <t>Siubtotal</t>
+  </si>
+  <si>
+    <t>Points</t>
+  </si>
+  <si>
+    <t>Subtotal</t>
   </si>
 </sst>
 </file>
@@ -166,7 +178,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -174,17 +186,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -499,317 +525,241 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7896AEF-34AA-E746-914C-B3A1A695E7D1}">
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17" customWidth="1"/>
+    <col min="1" max="1" width="46.83203125" customWidth="1"/>
+    <col min="2" max="2" width="5.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3">
-        <v>4</v>
-      </c>
-      <c r="C3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
-      <c r="C4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="B5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>7</v>
       </c>
-      <c r="B5">
-        <v>3</v>
-      </c>
-      <c r="C5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="B6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B6">
-        <v>3</v>
-      </c>
-      <c r="C6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
+      <c r="B7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="3">
-        <v>4</v>
-      </c>
-      <c r="C7" s="3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
-        <v>10</v>
-      </c>
       <c r="B8">
         <v>1</v>
       </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B9">
-        <v>2</v>
-      </c>
-      <c r="C9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="B10" s="3">
         <f>SUM(B3:B9)</f>
-        <v>20</v>
-      </c>
-      <c r="C10" s="3">
-        <f>SUM(C3:C9)</f>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+      <c r="D10" s="3"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="4">
-        <v>2</v>
-      </c>
-      <c r="C14" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
+      <c r="B15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="4">
-        <v>1</v>
-      </c>
-      <c r="C15" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16" s="4">
-        <v>3</v>
-      </c>
-      <c r="C16" s="4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="4">
-        <v>3</v>
-      </c>
-      <c r="C17" s="4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
+      <c r="B18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="4">
-        <v>3</v>
-      </c>
-      <c r="C18" s="4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="4" t="s">
+      <c r="B19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="4">
-        <v>3</v>
-      </c>
-      <c r="C19" s="4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="4" t="s">
+      <c r="B20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="4">
-        <v>2</v>
-      </c>
-      <c r="C20" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="4" t="s">
+      <c r="B21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="4">
-        <v>1</v>
-      </c>
-      <c r="C21" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="4" t="s">
+      <c r="B22">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B22" s="4">
-        <v>3</v>
-      </c>
-      <c r="C22" s="4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="4" t="s">
+      <c r="B25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B23" s="4">
-        <v>1</v>
-      </c>
-      <c r="C23" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B24" s="4">
-        <v>1</v>
-      </c>
-      <c r="C24" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B25" s="4">
-        <v>1</v>
-      </c>
-      <c r="C25" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B26" s="4">
-        <v>1</v>
-      </c>
-      <c r="C26" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B27" s="4">
-        <v>5</v>
-      </c>
-      <c r="C27" s="4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B27" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>3</v>
+        <v>28</v>
       </c>
       <c r="B28" s="3">
         <f>SUM(B14:B27)</f>
-        <v>30</v>
-      </c>
-      <c r="C28" s="3">
-        <f>SUM(C14:C27)</f>
-        <v>30</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B29" s="5">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D29" s="3"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B30" s="5">
         <f>SUM(B10,B28)</f>
-        <v>50</v>
-      </c>
-      <c r="C29" s="5">
-        <f>SUM(C10,C28)</f>
-        <v>50</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -819,10 +769,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96879333-0874-3847-ABBB-D0DF183A7724}">
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView zoomScale="156" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView topLeftCell="A20" zoomScale="156" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -834,7 +784,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -842,37 +792,37 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C3">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C4">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5">
         <v>3</v>
@@ -883,7 +833,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6">
         <v>3</v>
@@ -894,173 +844,173 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="3">
-        <v>5</v>
-      </c>
-      <c r="C7" s="3">
-        <v>5</v>
+        <v>8</v>
+      </c>
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C8">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" s="3">
-        <f>SUM(B3:B8)</f>
-        <v>20</v>
-      </c>
-      <c r="C9" s="3">
-        <f>SUM(C3:C8)</f>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>13</v>
+      <c r="A9" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="7">
+        <v>2</v>
+      </c>
+      <c r="C9" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="9">
+        <f>SUM(B3:B9)</f>
+        <v>15</v>
+      </c>
+      <c r="C10" s="9">
+        <f>SUM(C3:C9)</f>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" s="4">
-        <v>2</v>
-      </c>
-      <c r="C13" s="4">
+      <c r="B13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" s="4">
-        <v>1</v>
-      </c>
-      <c r="C14" s="4">
-        <v>1</v>
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14">
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="4">
-        <v>3</v>
-      </c>
-      <c r="C15" s="4">
-        <v>3</v>
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16" s="4">
-        <v>3</v>
-      </c>
-      <c r="C16" s="4">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>3</v>
+      </c>
+      <c r="C16">
         <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17" s="4">
-        <v>3</v>
-      </c>
-      <c r="C17" s="4">
-        <v>3</v>
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18" s="4">
-        <v>3</v>
-      </c>
-      <c r="C18" s="4">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>3</v>
+      </c>
+      <c r="C18">
         <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B19" s="4">
-        <v>2</v>
-      </c>
-      <c r="C19" s="4">
-        <v>2</v>
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>3</v>
+      </c>
+      <c r="C19">
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B20" s="4">
-        <v>1</v>
-      </c>
-      <c r="C20" s="4">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B21" s="4">
-        <v>3</v>
-      </c>
-      <c r="C21" s="4">
-        <v>3</v>
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B22" s="4">
-        <v>1</v>
-      </c>
-      <c r="C22" s="4">
-        <v>1</v>
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>3</v>
+      </c>
+      <c r="C22">
+        <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B23" s="4">
-        <v>1</v>
-      </c>
-      <c r="C23" s="4">
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
         <v>1</v>
       </c>
     </row>
@@ -1068,59 +1018,70 @@
       <c r="A24" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B24" s="4">
-        <v>1</v>
-      </c>
-      <c r="C24" s="4">
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24">
         <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B25" s="4">
-        <v>1</v>
-      </c>
-      <c r="C25" s="4">
+        <v>22</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25">
         <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B26" s="4">
-        <v>5</v>
-      </c>
-      <c r="C26" s="4">
-        <v>5</v>
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B27" s="3">
-        <f>SUM(B13:B26)</f>
-        <v>30</v>
-      </c>
-      <c r="C27" s="3">
-        <f>SUM(C13:C26)</f>
-        <v>30</v>
+      <c r="A27" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B27" s="7">
+        <v>2</v>
+      </c>
+      <c r="C27" s="7">
+        <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B28" s="5">
-        <f>SUM(B9,B27)</f>
-        <v>50</v>
-      </c>
-      <c r="C28" s="5">
-        <f>SUM(C9,C27)</f>
-        <v>50</v>
+      <c r="A28" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B28" s="3">
+        <f>SUM(B14:B27)</f>
+        <v>25</v>
+      </c>
+      <c r="C28" s="3">
+        <f>SUM(C14:C27)</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B29" s="5">
+        <f>SUM(B10,B28)</f>
+        <v>40</v>
+      </c>
+      <c r="C29" s="5">
+        <f>SUM(C10,C28)</f>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Minor update to rubric
</commit_message>
<xml_diff>
--- a/LabStarters/Lab06/Lab6Rubric-CIS195.xlsx
+++ b/LabStarters/Lab06/Lab6Rubric-CIS195.xlsx
@@ -1,32 +1,43 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DataCard/Repos/CIS195-CourseMaterials/LabStarters/Lab06/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\CIS195-CourseMaterials\LabStarters\Lab06\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C8D7005D-96B5-E24B-89C1-62C87A8D8F9C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FD14524-E858-4856-97C3-CCB462AE1A40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5960" yWindow="500" windowWidth="20920" windowHeight="16500" xr2:uid="{5D75B731-65CD-014E-8BBA-DE69945DF98D}"/>
+    <workbookView xWindow="18540" yWindow="3372" windowWidth="12156" windowHeight="12312" activeTab="1" xr2:uid="{5D75B731-65CD-014E-8BBA-DE69945DF98D}"/>
   </bookViews>
   <sheets>
     <sheet name="Rubric" sheetId="1" r:id="rId1"/>
     <sheet name="Student Scores" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="35">
   <si>
     <t>Requirements:</t>
   </si>
@@ -122,6 +133,15 @@
   </si>
   <si>
     <t>Subtotal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Each &lt;td&gt; has day of the month number </t>
+  </si>
+  <si>
+    <t>2+ events per day on different rows</t>
+  </si>
+  <si>
+    <t>A column for each day  (at least 5)</t>
   </si>
 </sst>
 </file>
@@ -199,18 +219,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -527,22 +542,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7896AEF-34AA-E746-914C-B3A1A695E7D1}">
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="46.83203125" customWidth="1"/>
+    <col min="1" max="1" width="46.796875" customWidth="1"/>
     <col min="2" max="2" width="5.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -550,7 +565,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -558,7 +573,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -566,7 +581,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -574,7 +589,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -582,31 +597,31 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>8</v>
       </c>
       <c r="B7">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>9</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="8" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B9" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>29</v>
       </c>
@@ -616,12 +631,12 @@
       </c>
       <c r="D10" s="3"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>0</v>
       </c>
@@ -629,119 +644,119 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>13</v>
       </c>
       <c r="B14">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>14</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="4" t="s">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>15</v>
       </c>
       <c r="B16">
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="4" t="s">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>27</v>
       </c>
       <c r="B17">
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>17</v>
       </c>
       <c r="B18">
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="4" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>18</v>
       </c>
       <c r="B19">
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="4" t="s">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>19</v>
       </c>
       <c r="B20">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="4" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>20</v>
       </c>
       <c r="B21">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="4" t="s">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
         <v>21</v>
       </c>
       <c r="B22">
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="4" t="s">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
         <v>24</v>
       </c>
       <c r="B23">
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="4" t="s">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
         <v>23</v>
       </c>
       <c r="B24">
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="4" t="s">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
         <v>22</v>
       </c>
       <c r="B25">
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="4" t="s">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
         <v>25</v>
       </c>
       <c r="B26">
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="8" t="s">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
         <v>4</v>
       </c>
-      <c r="B27" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B27" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>28</v>
       </c>
@@ -750,14 +765,14 @@
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D29" s="3"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B30" s="5">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B30" s="4">
         <f>SUM(B10,B28)</f>
         <v>40</v>
       </c>
@@ -771,23 +786,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96879333-0874-3847-ABBB-D0DF183A7724}">
   <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" zoomScale="156" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35" customWidth="1"/>
-    <col min="2" max="2" width="6.5" customWidth="1"/>
-    <col min="3" max="3" width="7.5" customWidth="1"/>
+    <col min="1" max="1" width="33.8984375" customWidth="1"/>
+    <col min="2" max="2" width="7" customWidth="1"/>
+    <col min="3" max="3" width="5.69921875" customWidth="1"/>
+    <col min="4" max="4" width="1.296875" customWidth="1"/>
+    <col min="5" max="5" width="23.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -798,9 +815,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -809,7 +826,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -820,7 +837,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -831,7 +848,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -842,9 +859,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
-        <v>8</v>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>33</v>
       </c>
       <c r="B7">
         <v>3</v>
@@ -853,8 +870,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>9</v>
       </c>
       <c r="B8">
@@ -864,36 +881,36 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="6" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="7">
-        <v>2</v>
-      </c>
-      <c r="C9" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="10" t="s">
+      <c r="B9" s="5">
+        <v>2</v>
+      </c>
+      <c r="C9" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="9">
+      <c r="B10">
         <f>SUM(B3:B9)</f>
         <v>15</v>
       </c>
-      <c r="C10" s="9">
+      <c r="C10">
         <f>SUM(C3:C9)</f>
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>0</v>
       </c>
@@ -904,8 +921,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>13</v>
       </c>
       <c r="B14">
@@ -915,8 +932,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>14</v>
       </c>
       <c r="B15">
@@ -926,9 +943,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="4" t="s">
-        <v>15</v>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>32</v>
       </c>
       <c r="B16">
         <v>3</v>
@@ -937,8 +954,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="4" t="s">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>16</v>
       </c>
       <c r="B17">
@@ -948,8 +965,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>17</v>
       </c>
       <c r="B18">
@@ -959,8 +976,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="4" t="s">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>18</v>
       </c>
       <c r="B19">
@@ -970,8 +987,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="4" t="s">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>19</v>
       </c>
       <c r="B20">
@@ -981,8 +998,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="4" t="s">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>20</v>
       </c>
       <c r="B21">
@@ -992,8 +1009,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="4" t="s">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
         <v>21</v>
       </c>
       <c r="B22">
@@ -1003,8 +1020,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="4" t="s">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
         <v>24</v>
       </c>
       <c r="B23">
@@ -1014,8 +1031,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="4" t="s">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
         <v>23</v>
       </c>
       <c r="B24">
@@ -1025,8 +1042,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="4" t="s">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
         <v>22</v>
       </c>
       <c r="B25">
@@ -1036,8 +1053,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="4" t="s">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
         <v>25</v>
       </c>
       <c r="B26">
@@ -1047,18 +1064,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" s="4" t="s">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
         <v>4</v>
       </c>
-      <c r="B27" s="7">
-        <v>2</v>
-      </c>
-      <c r="C27" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B27" s="5">
+        <v>2</v>
+      </c>
+      <c r="C27" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>3</v>
       </c>
@@ -1071,15 +1088,15 @@
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B29" s="5">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B29" s="4">
         <f>SUM(B10,B28)</f>
         <v>40</v>
       </c>
-      <c r="C29" s="5">
+      <c r="C29" s="4">
         <f>SUM(C10,C28)</f>
         <v>40</v>
       </c>

</xml_diff>